<commit_message>
Added file mover, sample size calculator and email sender scripts
</commit_message>
<xml_diff>
--- a/scripting & automation/sent_email_from_file/recipients.xlsx
+++ b/scripting & automation/sent_email_from_file/recipients.xlsx
@@ -38,10 +38,10 @@
     <t>Jane Micheal</t>
   </si>
   <si>
-    <t>juliandan7@gmail.com</t>
-  </si>
-  <si>
-    <t>simiyuwdan@gmail.com</t>
+    <t>simiyu.wdan32@gmail.com</t>
+  </si>
+  <si>
+    <t>julia.tyndan7@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +397,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -405,7 +405,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>